<commit_message>
fixing and adding 1 field change
</commit_message>
<xml_diff>
--- a/formb4b9.xlsx
+++ b/formb4b9.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LONG HẢI\Desktop\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C254C1A9-5E07-495E-8140-E95FE0402C66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4ACFE71-5FB7-45DF-A3BE-3C4FADBACB22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="912" yWindow="2172" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nội dung nhận xét" sheetId="1" r:id="rId1"/>
+    <sheet name="Thông tin GV" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="36">
   <si>
     <t>Tên GV</t>
   </si>
@@ -136,6 +137,9 @@
   </si>
   <si>
     <t>Tập trung hơn khi học</t>
+  </si>
+  <si>
+    <t>Ngày bắt đầu</t>
   </si>
 </sst>
 </file>
@@ -591,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K4" sqref="K4"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -630,21 +634,6 @@
       <c r="F1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G1" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" s="9" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="2" spans="1:11" ht="66" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
@@ -664,21 +653,6 @@
       </c>
       <c r="F2" s="5" t="s">
         <v>33</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" s="2">
-        <v>4</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="K2" s="12" t="s">
-        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="88.8" customHeight="1" x14ac:dyDescent="0.25">
@@ -786,4 +760,66 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0628467F-D81F-453E-AF08-E9CE1616A0EE}">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15.69921875" customWidth="1"/>
+    <col min="2" max="2" width="11.3984375" customWidth="1"/>
+    <col min="3" max="3" width="12.09765625" customWidth="1"/>
+    <col min="4" max="5" width="14.69921875" customWidth="1"/>
+    <col min="6" max="6" width="16.796875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2">
+        <v>4</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>